<commit_message>
Ajustes rotinas de inversão de datas trts 2 ao 12
</commit_message>
<xml_diff>
--- a/Data/Reports/AVON INDL LTDA.xlsx
+++ b/Data/Reports/AVON INDL LTDA.xlsx
@@ -4727,13 +4727,33 @@
       <c r="BT33" s="1" t="n"/>
     </row>
     <row r="34" ht="15.75" customHeight="1" s="18">
-      <c r="A34" s="32" t="n"/>
+      <c r="A34" s="32" t="inlineStr">
+        <is>
+          <t>00071</t>
+        </is>
+      </c>
       <c r="B34" s="32" t="n"/>
       <c r="C34" s="32" t="n"/>
-      <c r="D34" s="32" t="n"/>
-      <c r="E34" s="49" t="n"/>
-      <c r="F34" s="49" t="n"/>
-      <c r="G34" s="89" t="n"/>
+      <c r="D34" s="32" t="inlineStr">
+        <is>
+          <t>000000000235496</t>
+        </is>
+      </c>
+      <c r="E34" s="49" t="inlineStr">
+        <is>
+          <t>AVON INDL LTDA</t>
+        </is>
+      </c>
+      <c r="F34" s="49" t="inlineStr">
+        <is>
+          <t>MARCELO BASTOS DO NASCIMENTO</t>
+        </is>
+      </c>
+      <c r="G34" s="89" t="inlineStr">
+        <is>
+          <t>7.987,24</t>
+        </is>
+      </c>
       <c r="H34" s="34" t="n"/>
       <c r="I34" s="32" t="n"/>
       <c r="J34" s="32" t="n"/>
@@ -4758,11 +4778,27 @@
       <c r="AC34" s="38" t="n"/>
       <c r="AD34" s="38" t="n"/>
       <c r="AE34" s="38" t="n"/>
-      <c r="AF34" s="90" t="n"/>
-      <c r="AG34" s="90" t="n"/>
-      <c r="AH34" s="32" t="n"/>
+      <c r="AF34" s="90" t="inlineStr">
+        <is>
+          <t>09970502215507</t>
+        </is>
+      </c>
+      <c r="AG34" s="90" t="inlineStr">
+        <is>
+          <t>00000149866</t>
+        </is>
+      </c>
+      <c r="AH34" s="32" t="inlineStr">
+        <is>
+          <t>05/06/1995</t>
+        </is>
+      </c>
       <c r="AI34" s="32" t="n"/>
-      <c r="AJ34" s="32" t="n"/>
+      <c r="AJ34" s="32" t="inlineStr">
+        <is>
+          <t>12345223695</t>
+        </is>
+      </c>
       <c r="AK34" s="32" t="n"/>
       <c r="AL34" s="32" t="n"/>
       <c r="AM34" s="32" t="n"/>
@@ -4800,13 +4836,33 @@
       <c r="BT34" s="1" t="n"/>
     </row>
     <row r="35" ht="15.75" customHeight="1" s="18">
-      <c r="A35" s="32" t="n"/>
+      <c r="A35" s="32" t="inlineStr">
+        <is>
+          <t>00064</t>
+        </is>
+      </c>
       <c r="B35" s="32" t="n"/>
       <c r="C35" s="32" t="n"/>
-      <c r="D35" s="32" t="n"/>
-      <c r="E35" s="49" t="n"/>
-      <c r="F35" s="49" t="n"/>
-      <c r="G35" s="89" t="n"/>
+      <c r="D35" s="32" t="inlineStr">
+        <is>
+          <t>000000000000068</t>
+        </is>
+      </c>
+      <c r="E35" s="49" t="inlineStr">
+        <is>
+          <t>AVON INDL LTDA</t>
+        </is>
+      </c>
+      <c r="F35" s="49" t="inlineStr">
+        <is>
+          <t>PERCI ALESSANDRO RIBEIRO</t>
+        </is>
+      </c>
+      <c r="G35" s="89" t="inlineStr">
+        <is>
+          <t>7.786,05</t>
+        </is>
+      </c>
       <c r="H35" s="34" t="n"/>
       <c r="I35" s="32" t="n"/>
       <c r="J35" s="32" t="n"/>
@@ -4831,11 +4887,27 @@
       <c r="AC35" s="38" t="n"/>
       <c r="AD35" s="38" t="n"/>
       <c r="AE35" s="38" t="n"/>
-      <c r="AF35" s="90" t="n"/>
-      <c r="AG35" s="90" t="n"/>
-      <c r="AH35" s="32" t="n"/>
+      <c r="AF35" s="90" t="inlineStr">
+        <is>
+          <t>09970502215507</t>
+        </is>
+      </c>
+      <c r="AG35" s="90" t="inlineStr">
+        <is>
+          <t>00000154274</t>
+        </is>
+      </c>
+      <c r="AH35" s="32" t="inlineStr">
+        <is>
+          <t>11/03/1991</t>
+        </is>
+      </c>
       <c r="AI35" s="32" t="n"/>
-      <c r="AJ35" s="32" t="n"/>
+      <c r="AJ35" s="32" t="inlineStr">
+        <is>
+          <t>12340560359</t>
+        </is>
+      </c>
       <c r="AK35" s="32" t="n"/>
       <c r="AL35" s="32" t="n"/>
       <c r="AM35" s="32" t="n"/>
@@ -4873,13 +4945,33 @@
       <c r="BT35" s="1" t="n"/>
     </row>
     <row r="36" ht="15.75" customHeight="1" s="18">
-      <c r="A36" s="32" t="n"/>
+      <c r="A36" s="32" t="inlineStr">
+        <is>
+          <t>00004</t>
+        </is>
+      </c>
       <c r="B36" s="32" t="n"/>
       <c r="C36" s="32" t="n"/>
-      <c r="D36" s="32" t="n"/>
-      <c r="E36" s="49" t="n"/>
-      <c r="F36" s="49" t="n"/>
-      <c r="G36" s="89" t="n"/>
+      <c r="D36" s="32" t="inlineStr">
+        <is>
+          <t>000000122292012</t>
+        </is>
+      </c>
+      <c r="E36" s="49" t="inlineStr">
+        <is>
+          <t>AVON INDL LTDA</t>
+        </is>
+      </c>
+      <c r="F36" s="49" t="inlineStr">
+        <is>
+          <t>SILVANA APARECIDA CANOVA ARAUJO</t>
+        </is>
+      </c>
+      <c r="G36" s="89" t="inlineStr">
+        <is>
+          <t>8.802,15</t>
+        </is>
+      </c>
       <c r="H36" s="34" t="n"/>
       <c r="I36" s="32" t="n"/>
       <c r="J36" s="32" t="n"/>
@@ -4904,11 +4996,27 @@
       <c r="AC36" s="38" t="n"/>
       <c r="AD36" s="38" t="n"/>
       <c r="AE36" s="38" t="n"/>
-      <c r="AF36" s="90" t="n"/>
-      <c r="AG36" s="90" t="n"/>
-      <c r="AH36" s="32" t="n"/>
+      <c r="AF36" s="90" t="inlineStr">
+        <is>
+          <t>09970502215507</t>
+        </is>
+      </c>
+      <c r="AG36" s="90" t="inlineStr">
+        <is>
+          <t>00000751523</t>
+        </is>
+      </c>
+      <c r="AH36" s="32" t="inlineStr">
+        <is>
+          <t>18/07/2012</t>
+        </is>
+      </c>
       <c r="AI36" s="32" t="n"/>
-      <c r="AJ36" s="32" t="n"/>
+      <c r="AJ36" s="32" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
       <c r="AK36" s="32" t="n"/>
       <c r="AL36" s="32" t="n"/>
       <c r="AM36" s="32" t="n"/>
@@ -4946,13 +5054,33 @@
       <c r="BT36" s="1" t="n"/>
     </row>
     <row r="37" ht="15.75" customHeight="1" s="18">
-      <c r="A37" s="32" t="n"/>
+      <c r="A37" s="32" t="inlineStr">
+        <is>
+          <t>00077</t>
+        </is>
+      </c>
       <c r="B37" s="32" t="n"/>
       <c r="C37" s="32" t="n"/>
-      <c r="D37" s="32" t="n"/>
-      <c r="E37" s="49" t="n"/>
-      <c r="F37" s="49" t="n"/>
-      <c r="G37" s="89" t="n"/>
+      <c r="D37" s="32" t="inlineStr">
+        <is>
+          <t>000000002572000</t>
+        </is>
+      </c>
+      <c r="E37" s="49" t="inlineStr">
+        <is>
+          <t>AVON INDL LTDA</t>
+        </is>
+      </c>
+      <c r="F37" s="49" t="inlineStr">
+        <is>
+          <t>WILSON BEZERRA DOS SANTOS</t>
+        </is>
+      </c>
+      <c r="G37" s="89" t="inlineStr">
+        <is>
+          <t>7.325,46</t>
+        </is>
+      </c>
       <c r="H37" s="34" t="n"/>
       <c r="I37" s="32" t="n"/>
       <c r="J37" s="32" t="n"/>
@@ -4977,11 +5105,27 @@
       <c r="AC37" s="38" t="n"/>
       <c r="AD37" s="38" t="n"/>
       <c r="AE37" s="38" t="n"/>
-      <c r="AF37" s="90" t="n"/>
-      <c r="AG37" s="90" t="n"/>
-      <c r="AH37" s="32" t="n"/>
+      <c r="AF37" s="90" t="inlineStr">
+        <is>
+          <t>09970502215507</t>
+        </is>
+      </c>
+      <c r="AG37" s="90" t="inlineStr">
+        <is>
+          <t>00000246470</t>
+        </is>
+      </c>
+      <c r="AH37" s="32" t="inlineStr">
+        <is>
+          <t>02/05/1983</t>
+        </is>
+      </c>
       <c r="AI37" s="32" t="n"/>
-      <c r="AJ37" s="32" t="n"/>
+      <c r="AJ37" s="32" t="inlineStr">
+        <is>
+          <t>12010506784</t>
+        </is>
+      </c>
       <c r="AK37" s="32" t="n"/>
       <c r="AL37" s="32" t="n"/>
       <c r="AM37" s="32" t="n"/>

</xml_diff>